<commit_message>
I updated the feature file name
</commit_message>
<xml_diff>
--- a/reports/Extent-Report/Zlaata-QAResults.xlsx
+++ b/reports/Extent-Report/Zlaata-QAResults.xlsx
@@ -189,37 +189,37 @@
     <t>device</t>
   </si>
   <si>
-    <t>Oct 10, 2025 12:41:28 pm</t>
+    <t>Oct 10, 2025 1:24:50 pm</t>
   </si>
   <si>
-    <t>Oct 10, 2025 12:40:35 pm</t>
+    <t>Oct 10, 2025 1:24:34 pm</t>
   </si>
   <si>
-    <t>Oct 10, 2025 12:41:27 pm</t>
+    <t>Oct 10, 2025 1:24:49 pm</t>
   </si>
   <si>
-    <t>52.616 s</t>
+    <t>15.003 s</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
-    <t>TC_UI_Zlaata_PDP_02 | Verify  Discounted Price Calculating on Product details page | "TD_UI_Zlaata_PDP_02"</t>
+    <t>TC_UI_Zlaata_PLP_01 |Verify that the "Home" text link on the Product Listing page is clickable.|"TD_UI_Zlaata_PLP_01"</t>
   </si>
   <si>
-    <t>51.048 s</t>
+    <t>14.353 s</t>
   </si>
   <si>
-    <t>Product Details Page Feature</t>
+    <t>This is Product Listing Page feature</t>
   </si>
   <si>
-    <t>@TC_UI_Zlaata_PDP_02</t>
+    <t>@TC_UI_Zlaata_PLP_01</t>
   </si>
   <si>
     <t>@sanity</t>
   </si>
   <si>
-    <t>51.057 s</t>
+    <t>14.358 s</t>
   </si>
 </sst>
 </file>
@@ -1791,7 +1791,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_PDP_02 | Verify  Discounted Price Calculating on Product details page | "TD_UI_Zlaata_PDP_02"</c:v>
+                  <c:v>TC_UI_Zlaata_PLP_01 |Verify that the "Home" text link on the Product Listing page is clickable.|"TD_UI_Zlaata_PLP_01"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1863,7 +1863,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_PDP_02 | Verify  Discounted Price Calculating on Product details page | "TD_UI_Zlaata_PDP_02"</c:v>
+                  <c:v>TC_UI_Zlaata_PLP_01 |Verify that the "Home" text link on the Product Listing page is clickable.|"TD_UI_Zlaata_PLP_01"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1930,7 +1930,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_PDP_02 | Verify  Discounted Price Calculating on Product details page | "TD_UI_Zlaata_PDP_02"</c:v>
+                  <c:v>TC_UI_Zlaata_PLP_01 |Verify that the "Home" text link on the Product Listing page is clickable.|"TD_UI_Zlaata_PLP_01"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2337,7 +2337,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_PDP_02</c:v>
+                  <c:v>@TC_UI_Zlaata_PLP_01</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>@sanity</c:v>
@@ -2416,7 +2416,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_PDP_02</c:v>
+                  <c:v>@TC_UI_Zlaata_PLP_01</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>@sanity</c:v>
@@ -2487,7 +2487,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>@TC_UI_Zlaata_PDP_02</c:v>
+                  <c:v>@TC_UI_Zlaata_PLP_01</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>@sanity</c:v>
@@ -2706,7 +2706,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Product Details Page Feature</c:v>
+                  <c:v>This is Product Listing Page feature</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2778,7 +2778,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Product Details Page Feature</c:v>
+                  <c:v>This is Product Listing Page feature</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2845,7 +2845,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Product Details Page Feature</c:v>
+                  <c:v>This is Product Listing Page feature</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5788,7 +5788,7 @@
     <col min="7" max="7" customWidth="true" width="20.85546875"/>
   </cols>
   <sheetData/>
-  <sheetProtection sheet="true" password="B5F9" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="FC0D" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
New script for track inventories  import
</commit_message>
<xml_diff>
--- a/reports/Extent-Report/Zlaata-QAResults.xlsx
+++ b/reports/Extent-Report/Zlaata-QAResults.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>Duration</t>
   </si>
@@ -189,40 +189,34 @@
     <t>device</t>
   </si>
   <si>
-    <t>Dec 25, 2025 11:15:53 AM</t>
+    <t>Jan 02, 2026 5:03:57 pm</t>
   </si>
   <si>
-    <t>Dec 25, 2025 11:14:57 AM</t>
+    <t>Jan 02, 2026 5:03:21 pm</t>
   </si>
   <si>
-    <t>Dec 25, 2025 11:15:51 AM</t>
+    <t>Jan 02, 2026 5:03:56 pm</t>
   </si>
   <si>
-    <t>54.469 s</t>
+    <t>34.933 s</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
-    <t>TC_UI_Zlaata_ADM_04 |Verify Category Section Display on Website.| "TD_UI_Zlaata_ADM_04"</t>
+    <t>TC_UI_Zlaata_ADI_08 | Verify that uploaded track inventory appears in Admin and User App | "TD_UI_Zlaata_ADI_08"</t>
   </si>
   <si>
-    <t>53.470 s</t>
+    <t>34.158 s</t>
   </si>
   <si>
-    <t>Home Page Banner upload verification admin panel</t>
+    <t>Import Functionality Verify that different entities (Categories, Products, Product Styles, Search Keywords, Collections) can be successfully uploaded via Excel and are reflected in both Admin and User App.</t>
   </si>
   <si>
-    <t>@Home</t>
+    <t>@TC_UI_Zlaata_ADI_08</t>
   </si>
   <si>
-    <t>@Regression</t>
-  </si>
-  <si>
-    <t>@TC_UI_Zlaata_ADM_04</t>
-  </si>
-  <si>
-    <t>53.479 s</t>
+    <t>34.164 s</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1788,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ADM_04 |Verify Category Section Display on Website.| "TD_UI_Zlaata_ADM_04"</c:v>
+                  <c:v>TC_UI_Zlaata_ADI_08 | Verify that uploaded track inventory appears in Admin and User App | "TD_UI_Zlaata_ADI_08"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1805,7 +1799,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1866,7 +1860,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ADM_04 |Verify Category Section Display on Website.| "TD_UI_Zlaata_ADM_04"</c:v>
+                  <c:v>TC_UI_Zlaata_ADI_08 | Verify that uploaded track inventory appears in Admin and User App | "TD_UI_Zlaata_ADI_08"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1933,7 +1927,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TC_UI_Zlaata_ADM_04 |Verify Category Section Display on Website.| "TD_UI_Zlaata_ADM_04"</c:v>
+                  <c:v>TC_UI_Zlaata_ADI_08 | Verify that uploaded track inventory appears in Admin and User App | "TD_UI_Zlaata_ADI_08"</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2336,33 +2330,21 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$24</c:f>
+              <c:f>Tags!$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@Home</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>@Regression</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>@TC_UI_Zlaata_ADM_04</c:v>
+                  <c:v>@TC_UI_Zlaata_ADI_08</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$D$22:$D$24</c:f>
+              <c:f>Tags!$D$22</c:f>
               <c:numCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2421,24 +2403,18 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$24</c:f>
+              <c:f>Tags!$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@Home</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>@Regression</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>@TC_UI_Zlaata_ADM_04</c:v>
+                  <c:v>@TC_UI_Zlaata_ADI_08</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$F$22:$F$24</c:f>
+              <c:f>Tags!$F$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2495,24 +2471,18 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$24</c:f>
+              <c:f>Tags!$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>@Home</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>@Regression</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>@TC_UI_Zlaata_ADM_04</c:v>
+                  <c:v>@TC_UI_Zlaata_ADI_08</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$E$22:$E$24</c:f>
+              <c:f>Tags!$E$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2721,7 +2691,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Home Page Banner upload verification admin panel</c:v>
+                  <c:v>Import Functionality Verify that different entities (Categories, Products, Product Styles, Search Keywords, Collections) can be successfully uploaded via Excel and are reflected in both Admin and User App.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2793,7 +2763,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Home Page Banner upload verification admin panel</c:v>
+                  <c:v>Import Functionality Verify that different entities (Categories, Products, Product Styles, Search Keywords, Collections) can be successfully uploaded via Excel and are reflected in both Admin and User App.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2860,7 +2830,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Home Page Banner upload verification admin panel</c:v>
+                  <c:v>Import Functionality Verify that different entities (Categories, Products, Product Styles, Search Keywords, Collections) can be successfully uploaded via Excel and are reflected in both Admin and User App.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5803,7 +5773,7 @@
     <col min="7" max="7" customWidth="true" width="20.85546875"/>
   </cols>
   <sheetData/>
-  <sheetProtection sheet="true" password="F457" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="BB63" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5893,10 +5863,10 @@
         <v>29</v>
       </c>
       <c r="G22" s="57" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H22" s="58" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I22" s="59"/>
       <c r="J22" s="60"/>
@@ -5915,7 +5885,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B20:I31"/>
+  <dimension ref="B20:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -5977,118 +5947,48 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="57" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D23" s="58" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61" t="s">
-        <v>54</v>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="35" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="57" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D24" s="58" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="54" t="s">
+    <row r="27">
+      <c r="B27" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C27" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="62" t="s">
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="I29" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I31" s="55" t="s">
+      <c r="I27" s="55" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6185,7 +6085,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E22" s="57" t="n">
         <v>1.0</v>
@@ -6199,10 +6099,10 @@
         <v>54</v>
       </c>
       <c r="J22" s="57" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K22" s="58" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="L22" s="59"/>
       <c r="M22" s="60"/>
@@ -6281,7 +6181,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6350,7 +6250,7 @@
       </c>
       <c r="H5" t="n" s="0">
         <f>SUM(H2:H4)</f>
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>